<commit_message>
Changed Global Glider Cal sheet depth to 0
Cal sheet for some gliders was showing 0m for the depth and data was not
ingesting, corrected files as needed to 0 instead of 0m
</commit_message>
<xml_diff>
--- a/GP05MOAS-GL276/Omaha_Cal_Info_GP05MOAS-GL276_00001.xlsx
+++ b/GP05MOAS-GL276/Omaha_Cal_Info_GP05MOAS-GL276_00001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18270" windowHeight="8055" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18270" windowHeight="8055" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Ref Des</t>
   </si>
@@ -101,9 +101,6 @@
   </si>
   <si>
     <t>144° 48.32' W</t>
-  </si>
-  <si>
-    <t>0m</t>
   </si>
   <si>
     <t>MV1404</t>
@@ -796,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,21 +852,21 @@
         <v>9</v>
       </c>
       <c r="L1" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>26</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="15">
         <v>276</v>
@@ -890,11 +887,11 @@
       <c r="H2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="18">
+        <v>0</v>
+      </c>
+      <c r="J2" s="15" t="s">
         <v>22</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>23</v>
       </c>
       <c r="K2" s="15"/>
       <c r="L2" s="13">
@@ -934,7 +931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -976,7 +973,7 @@
     </row>
     <row r="3" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="6">
         <v>276</v>
@@ -988,12 +985,12 @@
         <v>276</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="9">
         <v>276</v>
@@ -1011,13 +1008,13 @@
         <v>140</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="23">
         <v>276</v>
@@ -1035,13 +1032,13 @@
         <v>700</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="23">
         <v>276</v>
@@ -1059,13 +1056,13 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="23">
         <v>276</v>
@@ -1083,13 +1080,13 @@
         <v>3.9E-2</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="6">
         <v>276</v>
@@ -1101,12 +1098,12 @@
         <v>12</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="6">
         <v>276</v>
@@ -1118,7 +1115,7 @@
         <v>104</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
redmine # 9229 Calibration sheets added/changed for GP05MOAS gliders GL276, GL361-GL365, GL453, GL523, GL525, GL537, PG514, PG515.
</commit_message>
<xml_diff>
--- a/GP05MOAS-GL276/Omaha_Cal_Info_GP05MOAS-GL276_00001.xlsx
+++ b/GP05MOAS-GL276/Omaha_Cal_Info_GP05MOAS-GL276_00001.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18270" windowHeight="8055" tabRatio="377"/>
+    <workbookView xWindow="10160" yWindow="7920" windowWidth="22840" windowHeight="9640" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,12 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$105</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$375</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -103,9 +108,6 @@
     <t>144° 48.32' W</t>
   </si>
   <si>
-    <t>MV1404</t>
-  </si>
-  <si>
     <t>Lat</t>
   </si>
   <si>
@@ -146,6 +148,9 @@
   </si>
   <si>
     <t>GP05MOAS-GL276-04-CTDGVM000</t>
+  </si>
+  <si>
+    <t>MV-1404</t>
   </si>
 </sst>
 </file>
@@ -156,7 +161,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -243,8 +248,36 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,6 +296,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -316,7 +355,7 @@
         <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -324,27 +363,29 @@
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -385,12 +426,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -416,8 +451,22 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 15" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
@@ -793,31 +842,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875"/>
-    <col min="10" max="10" width="12.7109375"/>
-    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="10" width="15.83203125" customWidth="1"/>
+    <col min="11" max="11" width="20.5" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="1026" width="8.7109375"/>
+    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -851,22 +891,22 @@
       <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="N1" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="O1" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:17" s="14" customFormat="1">
       <c r="A2" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="15">
         <v>276</v>
@@ -874,24 +914,26 @@
       <c r="C2" s="15">
         <v>1</v>
       </c>
-      <c r="D2" s="16">
-        <v>41803</v>
-      </c>
-      <c r="E2" s="17">
-        <v>0</v>
-      </c>
-      <c r="F2" s="16"/>
+      <c r="D2" s="27">
+        <v>41805</v>
+      </c>
+      <c r="E2" s="28">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="F2" s="27">
+        <v>42157</v>
+      </c>
       <c r="G2" s="15" t="s">
         <v>20</v>
       </c>
       <c r="H2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="18">
+      <c r="I2" s="16">
         <v>0</v>
       </c>
-      <c r="J2" s="15" t="s">
-        <v>22</v>
+      <c r="J2" s="25" t="s">
+        <v>36</v>
       </c>
       <c r="K2" s="15"/>
       <c r="L2" s="13">
@@ -902,28 +944,33 @@
         <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="E",1,-1))</f>
         <v>-144.80533333333332</v>
       </c>
-      <c r="N2" s="19">
+      <c r="N2" s="17">
         <v>41804</v>
       </c>
-      <c r="O2" s="19">
+      <c r="O2" s="17">
         <v>42146</v>
       </c>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+    </row>
+    <row r="3" spans="1:17">
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="4"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -931,27 +978,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125"/>
-    <col min="9" max="9" width="11.85546875"/>
-    <col min="10" max="10" width="14.42578125"/>
-    <col min="11" max="11" width="13.42578125"/>
-    <col min="12" max="1026" width="8.7109375"/>
+    <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.5" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="30">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -964,16 +1006,16 @@
       <c r="D1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
-        <v>33</v>
+    <row r="3" spans="1:10" s="6" customFormat="1">
+      <c r="A3" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="B3" s="6">
         <v>276</v>
@@ -985,12 +1027,12 @@
         <v>276</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="6" customFormat="1">
       <c r="A4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="9">
         <v>276</v>
@@ -1001,92 +1043,92 @@
       <c r="D4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="24">
         <v>140</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J4" s="12"/>
     </row>
-    <row r="5" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="6" customFormat="1">
       <c r="A5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="23">
+        <v>33</v>
+      </c>
+      <c r="B5" s="21">
         <v>276</v>
       </c>
       <c r="C5" s="9">
         <v>1</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="23">
         <v>700</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="6" customFormat="1">
       <c r="A6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="23">
+        <v>33</v>
+      </c>
+      <c r="B6" s="21">
         <v>276</v>
       </c>
       <c r="C6" s="9">
         <v>1</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="23" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="26">
-        <v>1.1299999999999999</v>
+        <v>1.0960000000000001</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="6" customFormat="1">
       <c r="A7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="23">
+        <v>33</v>
+      </c>
+      <c r="B7" s="21">
         <v>276</v>
       </c>
       <c r="C7" s="9">
         <v>1</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="23">
         <v>3.9E-2</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J7" s="12"/>
     </row>
-    <row r="8" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
-        <v>35</v>
+    <row r="8" spans="1:10" s="6" customFormat="1">
+      <c r="A8" s="20" t="s">
+        <v>34</v>
       </c>
       <c r="B8" s="6">
         <v>276</v>
@@ -1098,12 +1140,12 @@
         <v>12</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
-        <v>36</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="6" customFormat="1">
+      <c r="A9" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="B9" s="6">
         <v>276</v>
@@ -1115,15 +1157,20 @@
         <v>104</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="6" customFormat="1">
       <c r="C10" s="9"/>
       <c r="G10" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>